<commit_message>
Se avanza harto en el informe, solo faltan las curvas. Al codigo de check_vectors de le anade conteo de true positive, true negative, false positive % false negative para llenr la matriz de confusion
</commit_message>
<xml_diff>
--- a/Tarea 2/enunciado_informe/matriz_confusion.xlsx
+++ b/Tarea 2/enunciado_informe/matriz_confusion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="15">
   <si>
     <t>Actual Positive</t>
   </si>
@@ -52,13 +52,22 @@
   </si>
   <si>
     <t>recall -&gt;</t>
+  </si>
+  <si>
+    <t>undetermined</t>
+  </si>
+  <si>
+    <t>world</t>
+  </si>
+  <si>
+    <t>usa only</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,13 +91,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -100,10 +121,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -115,8 +137,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -133,16 +157,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1242060</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -151,7 +175,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5295900" y="1295400"/>
+          <a:off x="7757160" y="297180"/>
           <a:ext cx="4572000" cy="1257300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -538,16 +562,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="16.44140625" customWidth="1"/>
     <col min="5" max="5" width="19.77734375" customWidth="1"/>
@@ -671,6 +695,326 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C12" s="1"/>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="1">
+        <f>43+32+34+34+39+35+43+37+30+45</f>
+        <v>372</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <f>H12</f>
+        <v>372</v>
+      </c>
+      <c r="E13" s="1">
+        <f>H13</f>
+        <v>65</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="1">
+        <f>7+12+5+9+5+5+9+8+5</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <f>H14</f>
+        <v>277</v>
+      </c>
+      <c r="E14" s="1">
+        <f>H15</f>
+        <v>1286</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="1">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1">
+        <f>H12/(H12+H14)</f>
+        <v>0.57318952234206466</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="1">
+        <f>H12/(H12+H13)</f>
+        <v>0.85125858123569798</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C22" s="1"/>
+      <c r="D22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <f>H22</f>
+        <v>33</v>
+      </c>
+      <c r="E23" s="1">
+        <f>H23</f>
+        <v>7</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <f>H24</f>
+        <v>335</v>
+      </c>
+      <c r="E24" s="1">
+        <f>H25</f>
+        <v>1625</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="1">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="1">
+        <f>H22/(H22+H24)</f>
+        <v>8.9673913043478257E-2</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="1">
+        <f>H22/(H22+H23)</f>
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C32" s="1"/>
+      <c r="D32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" s="1">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C33" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <f>H32</f>
+        <v>800</v>
+      </c>
+      <c r="E33" s="1">
+        <f>H33</f>
+        <v>192</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="1">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <f>H34</f>
+        <v>150</v>
+      </c>
+      <c r="E34" s="1">
+        <f>H35</f>
+        <v>858</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H34" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" s="1">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="1">
+        <f>H32/(H32+H34)</f>
+        <v>0.84210526315789469</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="1">
+        <f>H32/(H32+H33)</f>
+        <v>0.80645161290322576</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="H38" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
se crea excel con los 10 splits para calcular el f-score, su precision y recall. Se crea otro excel para hacer la matriz de confusion
</commit_message>
<xml_diff>
--- a/Tarea 2/enunciado_informe/matriz_confusion.xlsx
+++ b/Tarea 2/enunciado_informe/matriz_confusion.xlsx
@@ -564,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>